<commit_message>
comeco da interface do whast
</commit_message>
<xml_diff>
--- a/banco/dados_ph_excel.xlsx
+++ b/banco/dados_ph_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1135,6 +1135,1356 @@
         <v>6.85</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:22:47</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>7.08</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:22:50</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>7.89</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:22:53</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>7.63</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:22:56</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>7.86</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:22:59</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:02</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:06</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>6.74</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:09</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:12</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>6.34</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:15</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>7.48</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:18</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>7.79</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:21</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>6.46</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:24</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>8.130000000000001</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:27</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:30</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>7.28</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:33</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:36</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>8.02</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:39</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>6.41</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:42</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>5.81</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:45</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:48</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>6.05</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:51</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:54</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>7.38</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:23:57</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>8.34</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:01</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:04</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>8.09</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:07</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>6.28</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:10</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>7.15</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:13</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>6.82</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:16</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>5.59</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:19</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>7.86</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:22</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>7.28</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:25</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>6.36</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:28</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>5.84</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:31</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>7.96</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:34</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:37</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>7.85</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:40</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>7.07</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:43</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>7.28</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:46</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>7.83</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:50</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>7.42</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:53</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:56</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>8.390000000000001</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:24:59</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:25:02</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>6.29</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:25:05</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>7.01</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:25:08</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>8.18</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:25:11</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>7.46</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:33:29</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:33:32</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>6.57</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:33:36</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>6.22</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:33:39</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>7.24</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:33:42</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>7.92</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:33:45</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:33:48</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>6.83</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:33:51</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>6.26</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:33:56</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:33:59</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>5.93</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:03</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>7.87</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:06</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:09</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>7.04</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:12</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>7.97</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:15</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>8.359999999999999</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:18</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:21</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>5.91</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:24</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>7.44</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:27</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:30</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>7.64</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:33</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:36</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>6.19</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:40</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>7.98</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:43</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>6.86</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:46</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>8.119999999999999</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:49</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:52</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>7.44</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:55</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>7.23</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:34:58</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>7.69</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:35:01</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>7.31</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:35:04</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:35:07</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>6.89</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:35:10</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>6.09</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:35:14</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>5.77</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:35:17</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>6.09</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:38:37</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>6.93</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:38:40</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:38:43</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>7.21</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:38:46</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>7.04</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:38:49</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:38:52</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>8.35</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:38:55</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:38:58</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>6.81</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:01</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>8.35</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:05</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>7.38</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:08</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>7.89</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:11</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>7.38</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:14</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>5.89</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:17</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>6.82</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:20</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:24</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>6.21</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:27</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>6.55</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:30</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>7.71</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:33</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>5.91</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:36</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>5.92</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:39</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:42</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>6.14</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:45</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:48</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>7.65</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:51</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:54</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:39:57</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>8.289999999999999</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:00</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>7.58</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:03</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>6.74</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:06</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>7.82</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:09</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>8.140000000000001</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:13</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>8.26</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:16</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>6.81</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:19</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:22</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:25</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:28</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>5.51</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:31</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:34</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>6.08</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:37</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>5.52</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:40</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>5.77</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:43</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>7.29</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:46</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>7.79</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:49</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>7.04</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:52</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>5.76</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:56</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>6.58</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:40:59</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>6.72</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:41:02</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
+        <v>8.380000000000001</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:41:05</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>7.53</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:41:08</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:41:11</t>
+        </is>
+      </c>
+      <c r="B204" t="n">
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2025-08-07 22:41:14</t>
+        </is>
+      </c>
+      <c r="B205" t="n">
+        <v>6.71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>